<commit_message>
updates new figures, complete ms draft v1
</commit_message>
<xml_diff>
--- a/Data/CTtests-arrowgobies_2019Lab2021field.xlsx
+++ b/Data/CTtests-arrowgobies_2019Lab2021field.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristakraskura/Github_repositories/KK_etal_gobies_tempVar_tempTol/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55CC624-3043-FA4D-8B1A-F7E2F6E97954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B9C256-5679-2549-89A4-A38DD75C5DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab-ALL tests" sheetId="19" r:id="rId1"/>
@@ -652,9 +652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D0870C-6093-FC42-B29E-1113A9012FFD}">
   <dimension ref="A1:W501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="139" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q228" sqref="Q228"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12320,7 +12320,7 @@
         <v>50</v>
       </c>
       <c r="R148">
-        <v>21.21</v>
+        <v>12.88</v>
       </c>
       <c r="S148" s="11">
         <f t="shared" si="19"/>

</xml_diff>